<commit_message>
update of norwegian stock
</commit_message>
<xml_diff>
--- a/metadata_vehicle_fleet.xlsx
+++ b/metadata_vehicle_fleet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/ericyo_ntnu_no/Documents/2020 Indecol/Batteries/VehicleFleetDatabase/vehicle_fleet_git_hub/vehicle_stock/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/ericyo_ntnu_no/Documents/VehicleFleetDatabase/vehicle_fleet_git_hub/vehicle_stock/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="114_{8783A492-6791-2144-922C-7AD3FA03F87D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{72795B8E-9C14-544A-863E-D07A0FB0449C}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="114_{8783A492-6791-2144-922C-7AD3FA03F87D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F4D99021-1154-A94D-8649-27CFB7B969EE}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="15960" firstSheet="2" activeTab="3" xr2:uid="{EC06436E-79EB-6C40-AACD-F805B686F2F9}"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="15840" firstSheet="5" activeTab="6" xr2:uid="{EC06436E-79EB-6C40-AACD-F805B686F2F9}"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="17" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2307" uniqueCount="1169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2330" uniqueCount="1179">
   <si>
     <t>sheet names</t>
   </si>
@@ -3522,9 +3522,6 @@
     <t>Other fuel</t>
   </si>
   <si>
-    <t>includes, hybrids, hydrogen, and non-petrol non-diesel fuels</t>
-  </si>
-  <si>
     <t>label</t>
   </si>
   <si>
@@ -3580,6 +3577,39 @@
   </si>
   <si>
     <t>southern europe</t>
+  </si>
+  <si>
+    <t>Statistics Norway</t>
+  </si>
+  <si>
+    <t>https://www.ssb.no/en/transport-og-reiseliv</t>
+  </si>
+  <si>
+    <t>vehicle registrations by class, some motor energy as well</t>
+  </si>
+  <si>
+    <t>occasionally included with tables</t>
+  </si>
+  <si>
+    <t>hybrid vehicles classed sometimes as other and sometimes as own class</t>
+  </si>
+  <si>
+    <t>sometimes includes, hybrids, hydrogen, and non-petrol non-diesel fuel</t>
+  </si>
+  <si>
+    <t>Hydrogen</t>
+  </si>
+  <si>
+    <t>Petrol hybrid, chargeable</t>
+  </si>
+  <si>
+    <t>Diesel hybrid, chargeable</t>
+  </si>
+  <si>
+    <t>Diesel hybrid, non-chargeable</t>
+  </si>
+  <si>
+    <t>Petrol hybrid, non-chargeable</t>
   </si>
 </sst>
 </file>
@@ -4191,6 +4221,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="14" xfId="9" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4218,7 +4249,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Data_Sheet1 (2)_1" xfId="9" xr:uid="{A05CF8FC-8E3B-B342-BDAE-37CAC6F37D1B}"/>
@@ -5319,9 +5349,11 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF85723-464A-064D-83CE-7377013504DF}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
@@ -5692,7 +5724,7 @@
       <c r="H16" s="56"/>
       <c r="I16" s="56"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:8">
       <c r="A17" s="56" t="s">
         <v>1009</v>
       </c>
@@ -5707,7 +5739,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:8">
       <c r="A18" s="56" t="s">
         <v>1080</v>
       </c>
@@ -5720,6 +5752,29 @@
       </c>
       <c r="E18" s="3" t="s">
         <v>1082</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>863</v>
+      </c>
+      <c r="B19" s="43" t="s">
+        <v>1168</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>552</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>1169</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>1170</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>1171</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>1172</v>
       </c>
     </row>
   </sheetData>
@@ -5744,6 +5799,7 @@
     <hyperlink ref="E16" r:id="rId18" xr:uid="{892D02C7-9CA1-0048-A5FB-6FB2845DDFB2}"/>
     <hyperlink ref="E17" r:id="rId19" xr:uid="{D253691A-06B5-BF43-883C-B4CFA4A116ED}"/>
     <hyperlink ref="E18" r:id="rId20" xr:uid="{A1DBE924-07F8-EE40-997A-E9AD71F0A258}"/>
+    <hyperlink ref="E19" r:id="rId21" xr:uid="{BE54A884-657F-844A-AA58-41A3679173D5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5766,12 +5822,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="105" t="s">
         <v>1083</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
       <c r="E1" s="56"/>
     </row>
     <row r="2" spans="1:5">
@@ -6741,11 +6797,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DBC143-CAD8-B649-A9B2-A245A722C481}">
   <dimension ref="A1:U290"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B273" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B159" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O291" sqref="O291"/>
+      <selection pane="bottomRight" activeCell="C172" sqref="C172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.83203125" defaultRowHeight="15"/>
@@ -15838,11 +15894,11 @@
         <v>955</v>
       </c>
       <c r="C290" s="46" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="D290" s="34"/>
-      <c r="E290" s="105"/>
-      <c r="M290" s="105">
+      <c r="E290" s="96"/>
+      <c r="M290" s="96">
         <v>150</v>
       </c>
       <c r="N290" s="11" t="s">
@@ -15852,7 +15908,7 @@
         <v>39</v>
       </c>
       <c r="P290" s="11" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
   </sheetData>
@@ -16204,7 +16260,7 @@
         <v>767</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="D1" s="80" t="s">
         <v>115</v>
@@ -16222,10 +16278,10 @@
         <v>779</v>
       </c>
       <c r="L1" s="52" t="s">
+        <v>1150</v>
+      </c>
+      <c r="M1" s="51" t="s">
         <v>1151</v>
-      </c>
-      <c r="M1" s="51" t="s">
-        <v>1152</v>
       </c>
       <c r="N1" s="51" t="s">
         <v>782</v>
@@ -16996,7 +17052,7 @@
         <v>861</v>
       </c>
       <c r="C25" s="56" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>862</v>
@@ -17025,13 +17081,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="56" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C26" s="56" t="s">
         <v>1154</v>
       </c>
-      <c r="C26" s="56" t="s">
+      <c r="D26" s="7" t="s">
         <v>1155</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>1156</v>
       </c>
       <c r="F26" s="56" t="s">
         <v>863</v>
@@ -17055,7 +17111,7 @@
         <v>865</v>
       </c>
       <c r="C27" s="56" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>866</v>
@@ -17081,13 +17137,13 @@
     <row r="28" spans="1:14" s="56" customFormat="1" ht="17">
       <c r="A28" s="5"/>
       <c r="B28" s="56" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C28" s="56" t="s">
         <v>1164</v>
       </c>
-      <c r="C28" s="56" t="s">
+      <c r="D28" s="7" t="s">
         <v>1165</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>1166</v>
       </c>
       <c r="F28" s="56" t="s">
         <v>863</v>
@@ -17110,7 +17166,7 @@
         <v>867</v>
       </c>
       <c r="C29" s="56" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="D29" s="16" t="s">
         <v>868</v>
@@ -17141,7 +17197,7 @@
         <v>869</v>
       </c>
       <c r="C30" s="56" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="D30" s="16" t="s">
         <v>870</v>
@@ -17172,7 +17228,7 @@
         <v>871</v>
       </c>
       <c r="C31" s="56" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="D31" s="16" t="s">
         <v>872</v>
@@ -17203,7 +17259,7 @@
         <v>873</v>
       </c>
       <c r="C32" s="56" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>874</v>
@@ -17234,7 +17290,7 @@
         <v>875</v>
       </c>
       <c r="C33" s="56" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>876</v>
@@ -17265,7 +17321,7 @@
         <v>877</v>
       </c>
       <c r="C34" s="56" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>878</v>
@@ -17602,7 +17658,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AFBCF10-B42A-8D46-BA7B-B4277EA43498}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -17974,7 +18032,7 @@
         <v>1148</v>
       </c>
       <c r="C22" t="s">
-        <v>1149</v>
+        <v>1173</v>
       </c>
       <c r="E22" t="s">
         <v>863</v>
@@ -17987,46 +18045,87 @@
       <c r="A23" s="56">
         <v>22</v>
       </c>
+      <c r="B23" s="94" t="s">
+        <v>1174</v>
+      </c>
+      <c r="E23" s="56" t="s">
+        <v>863</v>
+      </c>
+      <c r="G23" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="56">
         <v>23</v>
       </c>
+      <c r="B24" s="94" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E24" s="56" t="s">
+        <v>863</v>
+      </c>
+      <c r="G24" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="56">
         <v>24</v>
       </c>
+      <c r="B25" s="94" t="s">
+        <v>1176</v>
+      </c>
+      <c r="E25" s="56" t="s">
+        <v>863</v>
+      </c>
+      <c r="G25" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="56">
         <v>25</v>
       </c>
+      <c r="B26" s="94" t="s">
+        <v>1177</v>
+      </c>
+      <c r="E26" s="56" t="s">
+        <v>863</v>
+      </c>
+      <c r="G26" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="56">
         <v>26</v>
       </c>
+      <c r="B27" s="94" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E27" s="56" t="s">
+        <v>863</v>
+      </c>
+      <c r="G27" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="56">
-        <v>27</v>
-      </c>
+      <c r="A28" s="56"/>
+      <c r="E28" s="56"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="56">
-        <v>28</v>
-      </c>
+      <c r="A29" s="56"/>
+      <c r="E29" s="56"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="56">
-        <v>29</v>
-      </c>
+      <c r="A30" s="56"/>
+      <c r="E30" s="56"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="56">
-        <v>30</v>
-      </c>
+      <c r="A31" s="56"/>
+      <c r="E31" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18037,8 +18136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D915AA-E68F-004E-AC5F-6B6D3B0FE68C}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -18083,16 +18182,16 @@
       <c r="K1" s="56"/>
     </row>
     <row r="2" spans="1:11" s="64" customFormat="1" ht="11">
-      <c r="A2" s="96">
+      <c r="A2" s="97">
         <v>1</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="101" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="100" t="s">
+      <c r="C2" s="101" t="s">
         <v>890</v>
       </c>
-      <c r="D2" s="100"/>
+      <c r="D2" s="101"/>
       <c r="E2" s="88" t="s">
         <v>891</v>
       </c>
@@ -18108,10 +18207,10 @@
       <c r="K2" s="88"/>
     </row>
     <row r="3" spans="1:11" s="64" customFormat="1" ht="11">
-      <c r="A3" s="96"/>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
+      <c r="A3" s="97"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
       <c r="E3" s="88" t="s">
         <v>894</v>
       </c>
@@ -18127,10 +18226,10 @@
       <c r="K3" s="88"/>
     </row>
     <row r="4" spans="1:11" s="64" customFormat="1" ht="11">
-      <c r="A4" s="96"/>
-      <c r="B4" s="100"/>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
+      <c r="A4" s="97"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
       <c r="E4" s="88" t="s">
         <v>897</v>
       </c>
@@ -18146,10 +18245,10 @@
       <c r="K4" s="88"/>
     </row>
     <row r="5" spans="1:11" s="64" customFormat="1" ht="11">
-      <c r="A5" s="96"/>
-      <c r="B5" s="100"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
+      <c r="A5" s="97"/>
+      <c r="B5" s="101"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
       <c r="E5" s="88" t="s">
         <v>900</v>
       </c>
@@ -18165,10 +18264,10 @@
       <c r="K5" s="88"/>
     </row>
     <row r="6" spans="1:11" s="64" customFormat="1" ht="11">
-      <c r="A6" s="96"/>
-      <c r="B6" s="100"/>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
+      <c r="A6" s="97"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="101"/>
       <c r="E6" s="88" t="s">
         <v>903</v>
       </c>
@@ -18182,10 +18281,10 @@
       <c r="K6" s="88"/>
     </row>
     <row r="7" spans="1:11" s="64" customFormat="1" ht="11">
-      <c r="A7" s="96"/>
-      <c r="B7" s="100"/>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
+      <c r="A7" s="97"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
       <c r="E7" s="88" t="s">
         <v>905</v>
       </c>
@@ -18199,10 +18298,10 @@
       <c r="K7" s="88"/>
     </row>
     <row r="8" spans="1:11" s="66" customFormat="1" ht="12" thickBot="1">
-      <c r="A8" s="97"/>
-      <c r="B8" s="101"/>
-      <c r="C8" s="101"/>
-      <c r="D8" s="101"/>
+      <c r="A8" s="98"/>
+      <c r="B8" s="102"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="102"/>
       <c r="E8" s="89" t="s">
         <v>907</v>
       </c>
@@ -18216,16 +18315,16 @@
       <c r="K8" s="89"/>
     </row>
     <row r="9" spans="1:11" s="65" customFormat="1" ht="12" thickTop="1">
-      <c r="A9" s="98">
+      <c r="A9" s="99">
         <v>2</v>
       </c>
-      <c r="B9" s="102" t="s">
+      <c r="B9" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="102" t="s">
+      <c r="C9" s="103" t="s">
         <v>909</v>
       </c>
-      <c r="D9" s="102"/>
+      <c r="D9" s="103"/>
       <c r="E9" s="90" t="s">
         <v>910</v>
       </c>
@@ -18243,10 +18342,10 @@
       <c r="K9" s="90"/>
     </row>
     <row r="10" spans="1:11" s="64" customFormat="1" ht="11">
-      <c r="A10" s="96"/>
-      <c r="B10" s="100"/>
-      <c r="C10" s="100"/>
-      <c r="D10" s="100"/>
+      <c r="A10" s="97"/>
+      <c r="B10" s="101"/>
+      <c r="C10" s="101"/>
+      <c r="D10" s="101"/>
       <c r="E10" s="88"/>
       <c r="F10" s="88"/>
       <c r="G10" s="68">
@@ -18260,10 +18359,10 @@
       <c r="K10" s="88"/>
     </row>
     <row r="11" spans="1:11" s="66" customFormat="1" ht="12" thickBot="1">
-      <c r="A11" s="97"/>
-      <c r="B11" s="101"/>
-      <c r="C11" s="101"/>
-      <c r="D11" s="101"/>
+      <c r="A11" s="98"/>
+      <c r="B11" s="102"/>
+      <c r="C11" s="102"/>
+      <c r="D11" s="102"/>
       <c r="E11" s="89"/>
       <c r="F11" s="89"/>
       <c r="G11" s="69">
@@ -18279,16 +18378,16 @@
       <c r="K11" s="89"/>
     </row>
     <row r="12" spans="1:11" s="64" customFormat="1" ht="12" thickTop="1">
-      <c r="A12" s="99">
+      <c r="A12" s="100">
         <v>3</v>
       </c>
-      <c r="B12" s="103" t="s">
+      <c r="B12" s="104" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="103" t="s">
+      <c r="C12" s="104" t="s">
         <v>915</v>
       </c>
-      <c r="D12" s="103"/>
+      <c r="D12" s="104"/>
       <c r="E12" s="88" t="s">
         <v>916</v>
       </c>
@@ -18306,10 +18405,10 @@
       <c r="K12" s="88"/>
     </row>
     <row r="13" spans="1:11" s="64" customFormat="1" ht="11">
-      <c r="A13" s="96"/>
-      <c r="B13" s="100"/>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
+      <c r="A13" s="97"/>
+      <c r="B13" s="101"/>
+      <c r="C13" s="101"/>
+      <c r="D13" s="101"/>
       <c r="E13" s="88" t="s">
         <v>919</v>
       </c>
@@ -18327,10 +18426,10 @@
       <c r="K13" s="88"/>
     </row>
     <row r="14" spans="1:11" s="64" customFormat="1" ht="11">
-      <c r="A14" s="96"/>
-      <c r="B14" s="100"/>
-      <c r="C14" s="100"/>
-      <c r="D14" s="100"/>
+      <c r="A14" s="97"/>
+      <c r="B14" s="101"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="101"/>
       <c r="E14" s="88"/>
       <c r="F14" s="88"/>
       <c r="G14" s="68">
@@ -18344,10 +18443,10 @@
       <c r="K14" s="88"/>
     </row>
     <row r="15" spans="1:11" s="64" customFormat="1" ht="11">
-      <c r="A15" s="96"/>
-      <c r="B15" s="100"/>
-      <c r="C15" s="100"/>
-      <c r="D15" s="100"/>
+      <c r="A15" s="97"/>
+      <c r="B15" s="101"/>
+      <c r="C15" s="101"/>
+      <c r="D15" s="101"/>
       <c r="E15" s="88"/>
       <c r="F15" s="88"/>
       <c r="G15" s="68">
@@ -18361,10 +18460,10 @@
       <c r="K15" s="88"/>
     </row>
     <row r="16" spans="1:11" s="66" customFormat="1" ht="12" thickBot="1">
-      <c r="A16" s="97"/>
-      <c r="B16" s="101"/>
-      <c r="C16" s="101"/>
-      <c r="D16" s="101"/>
+      <c r="A16" s="98"/>
+      <c r="B16" s="102"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="102"/>
       <c r="E16" s="89"/>
       <c r="F16" s="89"/>
       <c r="G16" s="69">
@@ -18378,16 +18477,16 @@
       <c r="K16" s="89"/>
     </row>
     <row r="17" spans="1:10" s="65" customFormat="1" ht="12" thickTop="1">
-      <c r="A17" s="98">
+      <c r="A17" s="99">
         <v>4</v>
       </c>
-      <c r="B17" s="102" t="s">
+      <c r="B17" s="103" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="102" t="s">
+      <c r="C17" s="103" t="s">
         <v>925</v>
       </c>
-      <c r="D17" s="102"/>
+      <c r="D17" s="103"/>
       <c r="E17" s="90" t="s">
         <v>926</v>
       </c>
@@ -18404,10 +18503,10 @@
       <c r="J17" s="90"/>
     </row>
     <row r="18" spans="1:10" s="64" customFormat="1" ht="11">
-      <c r="A18" s="96"/>
-      <c r="B18" s="100"/>
-      <c r="C18" s="100"/>
-      <c r="D18" s="100"/>
+      <c r="A18" s="97"/>
+      <c r="B18" s="101"/>
+      <c r="C18" s="101"/>
+      <c r="D18" s="101"/>
       <c r="E18" s="88" t="s">
         <v>929</v>
       </c>
@@ -18424,10 +18523,10 @@
       <c r="J18" s="88"/>
     </row>
     <row r="19" spans="1:10" s="64" customFormat="1" ht="11">
-      <c r="A19" s="96"/>
-      <c r="B19" s="100"/>
-      <c r="C19" s="100"/>
-      <c r="D19" s="100"/>
+      <c r="A19" s="97"/>
+      <c r="B19" s="101"/>
+      <c r="C19" s="101"/>
+      <c r="D19" s="101"/>
       <c r="E19" s="88"/>
       <c r="F19" s="88"/>
       <c r="G19" s="68">
@@ -18440,10 +18539,10 @@
       <c r="J19" s="88"/>
     </row>
     <row r="20" spans="1:10" s="64" customFormat="1" ht="17" customHeight="1">
-      <c r="A20" s="96"/>
-      <c r="B20" s="100"/>
-      <c r="C20" s="100"/>
-      <c r="D20" s="100"/>
+      <c r="A20" s="97"/>
+      <c r="B20" s="101"/>
+      <c r="C20" s="101"/>
+      <c r="D20" s="101"/>
       <c r="E20" s="88"/>
       <c r="F20" s="88"/>
       <c r="G20" s="68">
@@ -18456,10 +18555,10 @@
       <c r="J20" s="88"/>
     </row>
     <row r="21" spans="1:10" s="66" customFormat="1" ht="12" thickBot="1">
-      <c r="A21" s="97"/>
-      <c r="B21" s="101"/>
-      <c r="C21" s="101"/>
-      <c r="D21" s="101"/>
+      <c r="A21" s="98"/>
+      <c r="B21" s="102"/>
+      <c r="C21" s="102"/>
+      <c r="D21" s="102"/>
       <c r="E21" s="89"/>
       <c r="F21" s="89"/>
       <c r="G21" s="69">
@@ -18472,16 +18571,16 @@
       <c r="J21" s="89"/>
     </row>
     <row r="22" spans="1:10" s="65" customFormat="1" ht="12" thickTop="1">
-      <c r="A22" s="98">
+      <c r="A22" s="99">
         <v>5</v>
       </c>
-      <c r="B22" s="102" t="s">
+      <c r="B22" s="103" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="102" t="s">
+      <c r="C22" s="103" t="s">
         <v>935</v>
       </c>
-      <c r="D22" s="102"/>
+      <c r="D22" s="103"/>
       <c r="E22" s="90" t="s">
         <v>936</v>
       </c>
@@ -18490,14 +18589,16 @@
       </c>
       <c r="G22" s="70"/>
       <c r="H22" s="90"/>
-      <c r="I22" s="90"/>
+      <c r="I22" s="88" t="s">
+        <v>940</v>
+      </c>
       <c r="J22" s="90"/>
     </row>
     <row r="23" spans="1:10" s="64" customFormat="1" ht="11">
-      <c r="A23" s="96"/>
-      <c r="B23" s="100"/>
-      <c r="C23" s="100"/>
-      <c r="D23" s="100"/>
+      <c r="A23" s="97"/>
+      <c r="B23" s="101"/>
+      <c r="C23" s="101"/>
+      <c r="D23" s="101"/>
       <c r="E23" s="88" t="s">
         <v>938</v>
       </c>
@@ -18506,14 +18607,13 @@
       </c>
       <c r="G23" s="68"/>
       <c r="H23" s="88"/>
-      <c r="I23" s="88"/>
       <c r="J23" s="88"/>
     </row>
     <row r="24" spans="1:10" s="66" customFormat="1" ht="12" thickBot="1">
-      <c r="A24" s="97"/>
-      <c r="B24" s="101"/>
-      <c r="C24" s="101"/>
-      <c r="D24" s="101"/>
+      <c r="A24" s="98"/>
+      <c r="B24" s="102"/>
+      <c r="C24" s="102"/>
+      <c r="D24" s="102"/>
       <c r="E24" s="89" t="s">
         <v>51</v>
       </c>
@@ -19143,15 +19243,15 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC6518AA-504D-4402-945F-65861D218FD0}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="98777117-b212-45e1-a88d-0f4f09175248"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>